<commit_message>
add kvcache per gpu in excel or console output
</commit_message>
<xml_diff>
--- a/metrics/ds_v3_decode_result.xlsx
+++ b/metrics/ds_v3_decode_result.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="性能分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Performance Analysis" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -72,7 +73,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -94,6 +95,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -459,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,24 +485,25 @@
     <col width="12" customWidth="1" min="14" max="14"/>
     <col width="12" customWidth="1" min="15" max="15"/>
     <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>性能分析报告: deepseek_v3 (DECODE)</t>
+          <t>Performance Analysis Report: deepseek_v3 (DECODE)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>算子名称</t>
+          <t>Operator Name</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>类型</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -530,47 +533,52 @@
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>输入</t>
+          <t>Input</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>输出</t>
+          <t>Output</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>权重</t>
+          <t>Weight</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>计算(us)</t>
+          <t>Compute(us)</t>
         </is>
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>内存(us)</t>
+          <t>Memory(us)</t>
         </is>
       </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>传输(us)</t>
+          <t>Transfer(us)</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
-          <t>单层理论延时(us)</t>
+          <t>Single Layer Latency(us)</t>
         </is>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>总时间(ms)</t>
+          <t>Total Time(ms)</t>
         </is>
       </c>
       <c r="P3" s="2" t="inlineStr">
         <is>
-          <t>占比(%)</t>
+          <t>Percent(%)</t>
+        </is>
+      </c>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>Weight/Single GPU All Layers</t>
         </is>
       </c>
     </row>
@@ -633,6 +641,9 @@
       <c r="P4" s="6" t="n">
         <v>0.7</v>
       </c>
+      <c r="Q4" s="4" t="n">
+        <v>923467776</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -693,6 +704,9 @@
       <c r="P5" s="6" t="n">
         <v>1.8</v>
       </c>
+      <c r="Q5" s="4" t="n">
+        <v>2302672896</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -753,6 +767,9 @@
       <c r="P6" s="6" t="n">
         <v>2.39</v>
       </c>
+      <c r="Q6" s="4" t="n">
+        <v>15990784</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -813,6 +830,9 @@
       <c r="P7" s="6" t="n">
         <v>2.39</v>
       </c>
+      <c r="Q7" s="4" t="n">
+        <v>15990784</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -873,6 +893,9 @@
       <c r="P8" s="6" t="n">
         <v>5.24</v>
       </c>
+      <c r="Q8" s="4" t="n">
+        <v>7163871232</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -933,6 +956,9 @@
       <c r="P9" s="6" t="n">
         <v>0.58</v>
       </c>
+      <c r="Q9" s="4" t="n">
+        <v>792723456</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -993,6 +1019,9 @@
       <c r="P10" s="6" t="n">
         <v>0.29</v>
       </c>
+      <c r="Q10" s="4" t="n">
+        <v>396361728</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -1053,6 +1082,9 @@
       <c r="P11" s="6" t="n">
         <v>0.39</v>
       </c>
+      <c r="Q11" s="4" t="n">
+        <v>425721856</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
@@ -1113,6 +1145,9 @@
       <c r="P12" s="6" t="n">
         <v>19.95</v>
       </c>
+      <c r="Q12" s="4" t="n">
+        <v>1702887424</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
@@ -1173,6 +1208,9 @@
       <c r="P13" s="6" t="n">
         <v>10.16</v>
       </c>
+      <c r="Q13" s="4" t="n">
+        <v>851443712</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
@@ -1233,6 +1271,9 @@
       <c r="P14" s="6" t="n">
         <v>1.27</v>
       </c>
+      <c r="Q14" s="4" t="n">
+        <v>1702887424</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -1293,6 +1334,9 @@
       <c r="P15" s="6" t="n">
         <v>0.66</v>
       </c>
+      <c r="Q15" s="4" t="n">
+        <v>851443712</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
@@ -1353,6 +1397,9 @@
       <c r="P16" s="6" t="n">
         <v>5.99</v>
       </c>
+      <c r="Q16" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
@@ -1413,6 +1460,9 @@
       <c r="P17" s="6" t="n">
         <v>2.99</v>
       </c>
+      <c r="Q17" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
@@ -1473,6 +1523,9 @@
       <c r="P18" s="6" t="n">
         <v>5.99</v>
       </c>
+      <c r="Q18" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
@@ -1489,7 +1542,7 @@
         <v>64</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>7168</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>7168</v>
@@ -1533,6 +1586,9 @@
       <c r="P19" s="6" t="n">
         <v>14.85</v>
       </c>
+      <c r="Q19" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
@@ -1549,7 +1605,7 @@
         <v>64</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>7168</v>
+        <v>0</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>7168</v>
@@ -1593,11 +1649,14 @@
       <c r="P20" s="6" t="n">
         <v>24.37</v>
       </c>
+      <c r="Q20" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="inlineStr">
         <is>
-          <t>计算时间 (ms)</t>
+          <t>Compute Time (ms)</t>
         </is>
       </c>
       <c r="B24" s="8" t="n">
@@ -1607,7 +1666,7 @@
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
         <is>
-          <t>内存时间 (ms)</t>
+          <t>Memory Time (ms)</t>
         </is>
       </c>
       <c r="B25" s="8" t="n">
@@ -1617,7 +1676,7 @@
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
-          <t>传输时间 (ms)</t>
+          <t>Transfer Time (ms)</t>
         </is>
       </c>
       <c r="B26" s="8" t="n">
@@ -1627,7 +1686,7 @@
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>总耗时 (ms)</t>
+          <t>Total Time (ms)</t>
         </is>
       </c>
       <c r="B27" s="8" t="n">
@@ -1637,12 +1696,12 @@
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
         <is>
-          <t>性能瓶颈</t>
+          <t>Performance Bottleneck</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>combine (总耗时: 18.804 ms)</t>
+          <t>combine (Total Time: 18.804 ms)</t>
         </is>
       </c>
     </row>
@@ -1659,16 +1718,36 @@
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
         <is>
-          <t>吞吐量TPS</t>
+          <t>Throughput TPS</t>
         </is>
       </c>
       <c r="B33" s="8" t="n">
         <v>813.157</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>Weight Memory/Single GPU (GB)</t>
+        </is>
+      </c>
+      <c r="B34" s="8" t="n">
+        <v>15.968</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="inlineStr">
+        <is>
+          <t>KV Cache Memory/Single GPU (GB)</t>
+        </is>
+      </c>
+      <c r="B35" s="9" t="n">
+        <v>3.3e-05</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>